<commit_message>
Atualizado por script em 02-12-2023 14:46
</commit_message>
<xml_diff>
--- a/2023/azerbaijan_premier-league_2023-2024.xlsx
+++ b/2023/azerbaijan_premier-league_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V70"/>
+  <dimension ref="A1:V71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6897,6 +6897,98 @@
         </is>
       </c>
     </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>azerbaijan</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>premier-league</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E71" s="2" t="n">
+        <v>45262.54166666666</v>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Araz</t>
+        </is>
+      </c>
+      <c r="G71" t="n">
+        <v>1</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>Sabail</t>
+        </is>
+      </c>
+      <c r="I71" t="n">
+        <v>1</v>
+      </c>
+      <c r="J71" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>01/12/2023 01:13</t>
+        </is>
+      </c>
+      <c r="L71" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>02/12/2023 12:57</t>
+        </is>
+      </c>
+      <c r="N71" t="n">
+        <v>3.22</v>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>01/12/2023 01:13</t>
+        </is>
+      </c>
+      <c r="P71" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="Q71" t="inlineStr">
+        <is>
+          <t>02/12/2023 12:57</t>
+        </is>
+      </c>
+      <c r="R71" t="n">
+        <v>4.06</v>
+      </c>
+      <c r="S71" t="inlineStr">
+        <is>
+          <t>01/12/2023 01:13</t>
+        </is>
+      </c>
+      <c r="T71" t="n">
+        <v>5.46</v>
+      </c>
+      <c r="U71" t="inlineStr">
+        <is>
+          <t>02/12/2023 12:57</t>
+        </is>
+      </c>
+      <c r="V71" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/azerbaijan/premier-league/araz-pfk-sabail/bajmtRZ9/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizado por script em 22-12-2023 14:45
</commit_message>
<xml_diff>
--- a/2023/azerbaijan_premier-league_2023-2024.xlsx
+++ b/2023/azerbaijan_premier-league_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V85"/>
+  <dimension ref="A1:V86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8277,6 +8277,98 @@
         </is>
       </c>
     </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>azerbaijan</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>premier-league</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E86" s="2" t="n">
+        <v>45282.54166666666</v>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Gabala</t>
+        </is>
+      </c>
+      <c r="G86" t="n">
+        <v>1</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>Sabah Baku</t>
+        </is>
+      </c>
+      <c r="I86" t="n">
+        <v>0</v>
+      </c>
+      <c r="J86" t="n">
+        <v>3.09</v>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>21/12/2023 01:12</t>
+        </is>
+      </c>
+      <c r="L86" t="n">
+        <v>3.94</v>
+      </c>
+      <c r="M86" t="inlineStr">
+        <is>
+          <t>22/12/2023 12:57</t>
+        </is>
+      </c>
+      <c r="N86" t="n">
+        <v>3.51</v>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>21/12/2023 01:12</t>
+        </is>
+      </c>
+      <c r="P86" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="Q86" t="inlineStr">
+        <is>
+          <t>22/12/2023 12:59</t>
+        </is>
+      </c>
+      <c r="R86" t="n">
+        <v>2.01</v>
+      </c>
+      <c r="S86" t="inlineStr">
+        <is>
+          <t>21/12/2023 01:12</t>
+        </is>
+      </c>
+      <c r="T86" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="U86" t="inlineStr">
+        <is>
+          <t>22/12/2023 12:59</t>
+        </is>
+      </c>
+      <c r="V86" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/azerbaijan/premier-league/gabala-sabah-baku/WU5AgyAQ/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>